<commit_message>
edit csdl product_category table
</commit_message>
<xml_diff>
--- a/csdl-shopping-cart.xlsx
+++ b/csdl-shopping-cart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVMASTER\DEV2206LM_SpringBoot\shopping-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A16CE6-E7D4-4DB2-8FFB-75E3A6DE17C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73743F12-6AE6-4497-A050-7003BBE4743C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91351D13-8343-4BE5-AE49-126D9A46B319}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="260">
   <si>
     <t>Id</t>
   </si>
@@ -813,6 +813,9 @@
   </si>
   <si>
     <t>Bảng liên kết nhãn với sản phẩm</t>
+  </si>
+  <si>
+    <t>Id duy nhất để xác định loại sản phẩm.</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1244,7 @@
   <dimension ref="B2:AZ30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1544,13 +1547,13 @@
         <v>103</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>201</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>108</v>
+        <v>259</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>0</v>
@@ -1659,13 +1662,13 @@
         <v>104</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>13</v>
@@ -1772,6 +1775,15 @@
       </c>
       <c r="T7" s="4" t="s">
         <v>105</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
edit csdl file excel
</commit_message>
<xml_diff>
--- a/csdl-shopping-cart.xlsx
+++ b/csdl-shopping-cart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVMASTER\DEV2206LM_SpringBoot\shopping-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73743F12-6AE6-4497-A050-7003BBE4743C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BA0F3A-C17D-431D-8DE8-22D2DF2457CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91351D13-8343-4BE5-AE49-126D9A46B319}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="260">
   <si>
     <t>Id</t>
   </si>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E867DBF7-62FE-4C81-BE5B-4B051B3412A0}">
   <dimension ref="B2:AZ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AU9" sqref="AU9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1547,10 +1547,10 @@
         <v>103</v>
       </c>
       <c r="V5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>259</v>
@@ -1601,10 +1601,10 @@
         <v>152</v>
       </c>
       <c r="AT5" s="3" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="AU5" s="3" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="AV5" s="3"/>
       <c r="AX5" s="3" t="s">
@@ -1716,10 +1716,10 @@
         <v>153</v>
       </c>
       <c r="AT6" s="3" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="AU6" s="3" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="AV6" s="3"/>
       <c r="AX6" s="3" t="s">
@@ -1830,6 +1830,13 @@
       <c r="AR7" s="4" t="s">
         <v>154</v>
       </c>
+      <c r="AT7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU7" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="AV7" s="3"/>
       <c r="AX7" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
update csdl and cart-item
</commit_message>
<xml_diff>
--- a/csdl-shopping-cart.xlsx
+++ b/csdl-shopping-cart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVMASTER\DEV2206LM_SpringBoot\shopping-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CDCED1-58D1-4B50-BBBB-AB2C30E12AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DE9F80-2CAA-4FBF-93E0-0ED4509DBC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91351D13-8343-4BE5-AE49-126D9A46B319}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="299">
   <si>
     <t>Id</t>
   </si>
@@ -925,6 +925,22 @@
     <t>CONSTRAINT `fk_cart_user`
     FOREIGN KEY (`user_id`)
     REFERENCES `shop`.`user` (`id`)</t>
+  </si>
+  <si>
+    <t>BIGINT NOT NULL</t>
+  </si>
+  <si>
+    <t>CONSTRAINT `fk_cart_item_product`
+    FOREIGN KEY (`product_id`)
+    REFERENCES `shop`.`product` (`id`)</t>
+  </si>
+  <si>
+    <t>CONSTRAINT `fk_cart_item_cart`
+  FOREIGN KEY (`cart_id`)
+  REFERENCES `shop`.`cart` (`id`)</t>
+  </si>
+  <si>
+    <t>thay sessionId thành cartId</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1071,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1132,14 +1148,17 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1455,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E867DBF7-62FE-4C81-BE5B-4B051B3412A0}">
-  <dimension ref="B2:CB30"/>
+  <dimension ref="B2:CE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AV7" sqref="AV7"/>
+    <sheetView tabSelected="1" topLeftCell="BG7" workbookViewId="0">
+      <selection activeCell="BK9" sqref="BK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1507,36 +1526,40 @@
     <col min="47" max="47" width="22.6640625" style="11" customWidth="1"/>
     <col min="48" max="48" width="32.33203125" style="11" customWidth="1"/>
     <col min="49" max="49" width="51.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="51.77734375" style="1" customWidth="1"/>
+    <col min="50" max="50" width="16.109375" style="1" customWidth="1"/>
     <col min="51" max="51" width="8.88671875" style="1"/>
     <col min="52" max="52" width="13.6640625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="16.33203125" style="1" customWidth="1"/>
-    <col min="54" max="55" width="45.21875" style="1" customWidth="1"/>
-    <col min="56" max="56" width="8.88671875" style="1"/>
-    <col min="57" max="57" width="16.21875" style="1" customWidth="1"/>
-    <col min="58" max="58" width="15.6640625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="44.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="44.77734375" style="1" customWidth="1"/>
-    <col min="61" max="61" width="8.88671875" style="1"/>
-    <col min="62" max="62" width="15.33203125" style="1" customWidth="1"/>
-    <col min="63" max="63" width="16.109375" style="1" customWidth="1"/>
-    <col min="64" max="64" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="33.109375" style="1" customWidth="1"/>
-    <col min="66" max="66" width="8.88671875" style="1"/>
-    <col min="67" max="67" width="14.21875" style="1" customWidth="1"/>
-    <col min="68" max="68" width="13.88671875" style="1" customWidth="1"/>
-    <col min="69" max="70" width="39.33203125" style="1" customWidth="1"/>
-    <col min="71" max="71" width="8.88671875" style="1"/>
-    <col min="72" max="72" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.77734375" style="1" customWidth="1"/>
-    <col min="74" max="75" width="11.6640625" style="1" customWidth="1"/>
-    <col min="76" max="76" width="8.88671875" style="1"/>
-    <col min="77" max="77" width="11.88671875" style="1" customWidth="1"/>
-    <col min="78" max="78" width="13" style="1" customWidth="1"/>
-    <col min="79" max="16384" width="8.88671875" style="1"/>
+    <col min="53" max="53" width="16.33203125" style="6" customWidth="1"/>
+    <col min="54" max="54" width="15.44140625" style="11" customWidth="1"/>
+    <col min="55" max="55" width="28.5546875" style="11" customWidth="1"/>
+    <col min="56" max="56" width="32.5546875" style="11" customWidth="1"/>
+    <col min="57" max="57" width="45.21875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="12.88671875" style="1" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="1"/>
+    <col min="60" max="60" width="16.21875" style="1" customWidth="1"/>
+    <col min="61" max="61" width="15.6640625" style="1" customWidth="1"/>
+    <col min="62" max="62" width="44.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="44.77734375" style="1" customWidth="1"/>
+    <col min="64" max="64" width="8.88671875" style="1"/>
+    <col min="65" max="65" width="15.33203125" style="1" customWidth="1"/>
+    <col min="66" max="66" width="16.109375" style="1" customWidth="1"/>
+    <col min="67" max="67" width="33.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="33.109375" style="1" customWidth="1"/>
+    <col min="69" max="69" width="8.88671875" style="1"/>
+    <col min="70" max="70" width="14.21875" style="1" customWidth="1"/>
+    <col min="71" max="71" width="13.88671875" style="1" customWidth="1"/>
+    <col min="72" max="73" width="39.33203125" style="1" customWidth="1"/>
+    <col min="74" max="74" width="8.88671875" style="1"/>
+    <col min="75" max="75" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.77734375" style="1" customWidth="1"/>
+    <col min="77" max="78" width="11.6640625" style="1" customWidth="1"/>
+    <col min="79" max="79" width="8.88671875" style="1"/>
+    <col min="80" max="80" width="11.88671875" style="1" customWidth="1"/>
+    <col min="81" max="81" width="13" style="1" customWidth="1"/>
+    <col min="82" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:80" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:83" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
         <v>228</v>
       </c>
@@ -1555,21 +1578,21 @@
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
       <c r="P2" s="9"/>
-      <c r="R2" s="30" t="s">
+      <c r="R2" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Z2" s="30" t="s">
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Z2" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
       <c r="AE2" s="29" t="s">
         <v>231</v>
       </c>
@@ -1599,39 +1622,42 @@
       </c>
       <c r="BA2" s="29"/>
       <c r="BB2" s="29"/>
-      <c r="BC2" s="9"/>
-      <c r="BE2" s="29" t="s">
+      <c r="BC2" s="29"/>
+      <c r="BD2" s="29"/>
+      <c r="BE2" s="29"/>
+      <c r="BF2" s="9"/>
+      <c r="BH2" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="BF2" s="29"/>
-      <c r="BG2" s="29"/>
-      <c r="BH2" s="9"/>
-      <c r="BJ2" s="29" t="s">
+      <c r="BI2" s="29"/>
+      <c r="BJ2" s="29"/>
+      <c r="BK2" s="9"/>
+      <c r="BM2" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="BK2" s="29"/>
-      <c r="BL2" s="29"/>
-      <c r="BM2" s="9"/>
-      <c r="BO2" s="29" t="s">
+      <c r="BN2" s="29"/>
+      <c r="BO2" s="29"/>
+      <c r="BP2" s="9"/>
+      <c r="BR2" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="BP2" s="29"/>
-      <c r="BQ2" s="29"/>
-      <c r="BR2" s="9"/>
-      <c r="BT2" s="29" t="s">
+      <c r="BS2" s="29"/>
+      <c r="BT2" s="29"/>
+      <c r="BU2" s="9"/>
+      <c r="BW2" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="BU2" s="29"/>
-      <c r="BV2" s="29"/>
-      <c r="BW2" s="9"/>
-      <c r="BY2" s="29" t="s">
+      <c r="BX2" s="29"/>
+      <c r="BY2" s="29"/>
+      <c r="BZ2" s="9"/>
+      <c r="CB2" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="BZ2" s="29"/>
-      <c r="CA2" s="29"/>
-      <c r="CB2" s="9"/>
+      <c r="CC2" s="29"/>
+      <c r="CD2" s="29"/>
+      <c r="CE2" s="9"/>
     </row>
-    <row r="3" spans="2:80" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:83" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
@@ -1706,49 +1732,52 @@
       <c r="AZ3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="BA3" s="7"/>
-      <c r="BB3" s="7" t="s">
+      <c r="BA3" s="31"/>
+      <c r="BB3" s="12"/>
+      <c r="BC3" s="12"/>
+      <c r="BD3" s="12"/>
+      <c r="BE3" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="BC3" s="7"/>
-      <c r="BE3" s="8" t="s">
+      <c r="BF3" s="7"/>
+      <c r="BH3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="BF3" s="8"/>
-      <c r="BG3" s="8" t="s">
+      <c r="BI3" s="8"/>
+      <c r="BJ3" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="BH3" s="8"/>
-      <c r="BJ3" s="7" t="s">
+      <c r="BK3" s="8"/>
+      <c r="BM3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BK3" s="7"/>
-      <c r="BL3" s="7" t="s">
+      <c r="BN3" s="7"/>
+      <c r="BO3" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="BM3" s="7"/>
-      <c r="BO3" s="7" t="s">
+      <c r="BP3" s="7"/>
+      <c r="BR3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="BP3" s="7"/>
-      <c r="BQ3" s="7" t="s">
+      <c r="BS3" s="7"/>
+      <c r="BT3" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="BR3" s="7"/>
-      <c r="BT3" s="28" t="s">
+      <c r="BU3" s="7"/>
+      <c r="BW3" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="BU3" s="28"/>
-      <c r="BV3" s="28"/>
-      <c r="BW3" s="2"/>
-      <c r="BY3" s="28" t="s">
+      <c r="BX3" s="30"/>
+      <c r="BY3" s="30"/>
+      <c r="BZ3" s="2"/>
+      <c r="CB3" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="BZ3" s="28"/>
-      <c r="CA3" s="28"/>
-      <c r="CB3" s="2"/>
+      <c r="CC3" s="30"/>
+      <c r="CD3" s="30"/>
+      <c r="CE3" s="2"/>
     </row>
-    <row r="4" spans="2:80" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:83" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="18"/>
       <c r="C4" s="18" t="s">
         <v>280</v>
@@ -1833,31 +1862,42 @@
       <c r="AW4" s="18"/>
       <c r="AX4" s="21"/>
       <c r="AZ4" s="18"/>
-      <c r="BA4" s="18"/>
-      <c r="BB4" s="18"/>
-      <c r="BC4" s="21"/>
-      <c r="BE4" s="20"/>
-      <c r="BF4" s="20"/>
-      <c r="BG4" s="20"/>
-      <c r="BH4" s="23"/>
-      <c r="BJ4" s="18"/>
-      <c r="BK4" s="18"/>
-      <c r="BL4" s="18"/>
-      <c r="BM4" s="21"/>
+      <c r="BA4" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="BB4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC4" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="BD4" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="BE4" s="18"/>
+      <c r="BF4" s="21"/>
+      <c r="BH4" s="20"/>
+      <c r="BI4" s="20"/>
+      <c r="BJ4" s="20"/>
+      <c r="BK4" s="23"/>
+      <c r="BM4" s="18"/>
+      <c r="BN4" s="18"/>
       <c r="BO4" s="18"/>
-      <c r="BP4" s="18"/>
-      <c r="BQ4" s="18"/>
-      <c r="BR4" s="21"/>
+      <c r="BP4" s="21"/>
+      <c r="BR4" s="18"/>
+      <c r="BS4" s="18"/>
       <c r="BT4" s="18"/>
-      <c r="BU4" s="18"/>
-      <c r="BV4" s="18"/>
-      <c r="BW4" s="21"/>
+      <c r="BU4" s="21"/>
+      <c r="BW4" s="18"/>
+      <c r="BX4" s="18"/>
       <c r="BY4" s="18"/>
-      <c r="BZ4" s="18"/>
-      <c r="CA4" s="18"/>
-      <c r="CB4" s="21"/>
+      <c r="BZ4" s="21"/>
+      <c r="CB4" s="18"/>
+      <c r="CC4" s="18"/>
+      <c r="CD4" s="18"/>
+      <c r="CE4" s="21"/>
     </row>
-    <row r="5" spans="2:80" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:83" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
@@ -1970,61 +2010,70 @@
       <c r="AZ5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="BA5" s="14" t="s">
+      <c r="BA5" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="BB5" s="17" t="s">
+      <c r="BB5" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="BC5" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="BD5" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="BE5" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="BC5" s="10"/>
-      <c r="BE5" s="14" t="s">
+      <c r="BF5" s="10"/>
+      <c r="BH5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="BF5" s="14" t="s">
+      <c r="BI5" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="BG5" s="17" t="s">
+      <c r="BJ5" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="BH5" s="22"/>
-      <c r="BJ5" s="14" t="s">
+      <c r="BK5" s="10"/>
+      <c r="BM5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="BK5" s="14" t="s">
+      <c r="BN5" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="BL5" s="17" t="s">
+      <c r="BO5" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="BM5" s="22"/>
-      <c r="BO5" s="14" t="s">
+      <c r="BP5" s="22"/>
+      <c r="BR5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="BP5" s="14" t="s">
+      <c r="BS5" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="BQ5" s="17" t="s">
+      <c r="BT5" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="BR5" s="22"/>
-      <c r="BT5" s="14" t="s">
+      <c r="BU5" s="22"/>
+      <c r="BW5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="BU5" s="14" t="s">
+      <c r="BX5" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="BV5" s="14"/>
-      <c r="BW5" s="24"/>
-      <c r="BY5" s="14" t="s">
+      <c r="BY5" s="14"/>
+      <c r="BZ5" s="24"/>
+      <c r="CB5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="BZ5" s="14" t="s">
+      <c r="CC5" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="CA5" s="14"/>
-      <c r="CB5" s="24"/>
+      <c r="CD5" s="14"/>
+      <c r="CE5" s="24"/>
     </row>
-    <row r="6" spans="2:80" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:83" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2131,61 +2180,70 @@
       <c r="AZ6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BA6" s="3" t="s">
+      <c r="BA6" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="BB6" s="4" t="s">
+      <c r="BB6" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="BC6" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="BD6" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="BE6" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="BC6" s="10"/>
-      <c r="BE6" s="3" t="s">
+      <c r="BF6" s="10"/>
+      <c r="BH6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BF6" s="3" t="s">
+      <c r="BI6" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="BG6" s="4" t="s">
+      <c r="BJ6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="BH6" s="22"/>
-      <c r="BJ6" s="3" t="s">
+      <c r="BK6" s="10"/>
+      <c r="BM6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BK6" s="3" t="s">
+      <c r="BN6" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BL6" s="4" t="s">
+      <c r="BO6" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="BM6" s="22"/>
-      <c r="BO6" s="3" t="s">
+      <c r="BP6" s="22"/>
+      <c r="BR6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BP6" s="3" t="s">
+      <c r="BS6" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="BQ6" s="4" t="s">
+      <c r="BT6" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="BR6" s="22"/>
-      <c r="BT6" s="3" t="s">
+      <c r="BU6" s="22"/>
+      <c r="BW6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BU6" s="3" t="s">
+      <c r="BX6" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="BV6" s="3"/>
-      <c r="BW6" s="24"/>
-      <c r="BY6" s="3" t="s">
+      <c r="BY6" s="3"/>
+      <c r="BZ6" s="24"/>
+      <c r="CB6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="BZ6" s="3" t="s">
+      <c r="CC6" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="CA6" s="3"/>
-      <c r="CB6" s="24"/>
+      <c r="CD6" s="3"/>
+      <c r="CE6" s="24"/>
     </row>
-    <row r="7" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -2270,81 +2328,94 @@
         <v>107</v>
       </c>
       <c r="AP7" s="10"/>
-      <c r="AR7" s="3" t="s">
+      <c r="AR7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AS7" s="3" t="s">
+      <c r="AS7" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="AT7" s="10" t="s">
+      <c r="AT7" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="AU7" s="10" t="s">
+      <c r="AU7" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="AV7" s="10"/>
-      <c r="AW7" s="4" t="s">
+      <c r="AV7" s="26"/>
+      <c r="AW7" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="AX7" s="10"/>
+      <c r="AX7" s="26" t="s">
+        <v>291</v>
+      </c>
       <c r="AZ7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="BA7" s="3" t="s">
+      <c r="BA7" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="BB7" s="4" t="s">
+      <c r="BB7" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="BC7" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="BD7" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="BE7" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="BC7" s="10"/>
-      <c r="BE7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="BF7" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="BG7" s="4" t="s">
+      <c r="BF7" s="10"/>
+      <c r="BH7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI7" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="BJ7" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="BH7" s="22"/>
-      <c r="BJ7" s="3" t="s">
+      <c r="BK7" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="BM7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BK7" s="3" t="s">
+      <c r="BN7" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="BL7" s="4" t="s">
+      <c r="BO7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="BM7" s="22"/>
-      <c r="BO7" s="3" t="s">
+      <c r="BP7" s="22"/>
+      <c r="BR7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BP7" s="3" t="s">
+      <c r="BS7" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="BQ7" s="4" t="s">
+      <c r="BT7" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="BR7" s="22"/>
-      <c r="BT7" s="3" t="s">
+      <c r="BU7" s="22"/>
+      <c r="BW7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="BU7" s="3" t="s">
+      <c r="BX7" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="BV7" s="3"/>
-      <c r="BW7" s="24"/>
-      <c r="BY7" s="3" t="s">
+      <c r="BY7" s="3"/>
+      <c r="BZ7" s="24"/>
+      <c r="CB7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="BZ7" s="3" t="s">
+      <c r="CC7" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="CA7" s="3"/>
-      <c r="CB7" s="24"/>
+      <c r="CD7" s="3"/>
+      <c r="CE7" s="24"/>
     </row>
-    <row r="8" spans="2:80" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:83" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
@@ -2445,53 +2516,62 @@
       <c r="AZ8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BA8" s="3" t="s">
+      <c r="BA8" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="BB8" s="4" t="s">
+      <c r="BB8" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="BC8" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="BD8" s="10"/>
+      <c r="BE8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="BC8" s="10"/>
-      <c r="BE8" s="3" t="s">
+      <c r="BF8" s="10"/>
+      <c r="BH8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="BF8" s="3" t="s">
+      <c r="BI8" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="BG8" s="4" t="s">
+      <c r="BJ8" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="BH8" s="22"/>
-      <c r="BJ8" s="3" t="s">
+      <c r="BK8" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="BM8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BK8" s="3" t="s">
+      <c r="BN8" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="BL8" s="4" t="s">
+      <c r="BO8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="BM8" s="22"/>
-      <c r="BO8" s="3" t="s">
+      <c r="BP8" s="22"/>
+      <c r="BR8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="BP8" s="3" t="s">
+      <c r="BS8" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="BQ8" s="4" t="s">
+      <c r="BT8" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="BR8" s="22"/>
-      <c r="BY8" s="3" t="s">
+      <c r="BU8" s="22"/>
+      <c r="CB8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BZ8" s="3" t="s">
+      <c r="CC8" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="CA8" s="3"/>
-      <c r="CB8" s="24"/>
+      <c r="CD8" s="3"/>
+      <c r="CE8" s="24"/>
     </row>
-    <row r="9" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -2577,53 +2657,60 @@
       <c r="AZ9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BA9" s="3" t="s">
+      <c r="BA9" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="BB9" s="4" t="s">
+      <c r="BB9" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="BC9" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="BD9" s="10"/>
+      <c r="BE9" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="BC9" s="10"/>
-      <c r="BE9" s="3" t="s">
+      <c r="BF9" s="10"/>
+      <c r="BH9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="BF9" s="3" t="s">
+      <c r="BI9" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="BG9" s="4" t="s">
+      <c r="BJ9" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="BH9" s="22"/>
-      <c r="BJ9" s="3" t="s">
+      <c r="BK9" s="10"/>
+      <c r="BM9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BK9" s="3" t="s">
+      <c r="BN9" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="BL9" s="4" t="s">
+      <c r="BO9" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="BM9" s="22"/>
-      <c r="BO9" s="3" t="s">
+      <c r="BP9" s="22"/>
+      <c r="BR9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BP9" s="3" t="s">
+      <c r="BS9" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="BQ9" s="4" t="s">
+      <c r="BT9" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="BR9" s="22"/>
-      <c r="BY9" s="3" t="s">
+      <c r="BU9" s="22"/>
+      <c r="CB9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BZ9" s="3" t="s">
+      <c r="CC9" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="CA9" s="3"/>
-      <c r="CB9" s="24"/>
+      <c r="CD9" s="3"/>
+      <c r="CE9" s="24"/>
     </row>
-    <row r="10" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>167</v>
       </c>
@@ -2705,45 +2792,52 @@
       <c r="AZ10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="BA10" s="3" t="s">
+      <c r="BA10" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="BB10" s="4" t="s">
+      <c r="BB10" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="BC10" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="BD10" s="10"/>
+      <c r="BE10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="BC10" s="10"/>
-      <c r="BE10" s="3" t="s">
+      <c r="BF10" s="10"/>
+      <c r="BH10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BF10" s="3" t="s">
+      <c r="BI10" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="BG10" s="4" t="s">
+      <c r="BJ10" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="BH10" s="22"/>
-      <c r="BJ10" s="3" t="s">
+      <c r="BK10" s="10"/>
+      <c r="BM10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="BK10" s="3" t="s">
+      <c r="BN10" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="BL10" s="4" t="s">
+      <c r="BO10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="BM10" s="22"/>
-      <c r="BO10" s="3" t="s">
+      <c r="BP10" s="22"/>
+      <c r="BR10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BP10" s="3" t="s">
+      <c r="BS10" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="BQ10" s="4" t="s">
+      <c r="BT10" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BR10" s="22"/>
+      <c r="BU10" s="22"/>
     </row>
-    <row r="11" spans="2:80" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:83" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -2810,45 +2904,52 @@
       <c r="AZ11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="BA11" s="3" t="s">
+      <c r="BA11" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="BB11" s="4" t="s">
+      <c r="BB11" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC11" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="BD11" s="10"/>
+      <c r="BE11" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BC11" s="10"/>
-      <c r="BE11" s="3" t="s">
+      <c r="BF11" s="10"/>
+      <c r="BH11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="BF11" s="3" t="s">
+      <c r="BI11" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="BG11" s="4" t="s">
+      <c r="BJ11" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="BH11" s="22"/>
-      <c r="BJ11" s="3" t="s">
+      <c r="BK11" s="10"/>
+      <c r="BM11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="BK11" s="3" t="s">
+      <c r="BN11" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="BL11" s="4" t="s">
+      <c r="BO11" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BM11" s="22"/>
-      <c r="BO11" s="3" t="s">
+      <c r="BP11" s="22"/>
+      <c r="BR11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="BP11" s="3" t="s">
+      <c r="BS11" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="BQ11" s="4" t="s">
+      <c r="BT11" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="BR11" s="22"/>
+      <c r="BU11" s="22"/>
     </row>
-    <row r="12" spans="2:80" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:83" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2915,45 +3016,54 @@
       <c r="AZ12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="BA12" s="3" t="s">
+      <c r="BA12" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="BB12" s="4" t="s">
+      <c r="BB12" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="BC12" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="BD12" s="10"/>
+      <c r="BE12" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="BC12" s="10"/>
-      <c r="BE12" s="3" t="s">
+      <c r="BF12" s="10"/>
+      <c r="BH12" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="BF12" s="3" t="s">
+      <c r="BI12" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="BG12" s="4" t="s">
+      <c r="BJ12" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="BH12" s="22"/>
-      <c r="BJ12" s="3" t="s">
+      <c r="BK12" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="BM12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BK12" s="3" t="s">
+      <c r="BN12" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="BL12" s="4" t="s">
+      <c r="BO12" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="BM12" s="22"/>
-      <c r="BO12" s="3" t="s">
+      <c r="BP12" s="22"/>
+      <c r="BR12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BP12" s="3" t="s">
+      <c r="BS12" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="BQ12" s="4" t="s">
+      <c r="BT12" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="BR12" s="22"/>
+      <c r="BU12" s="22"/>
     </row>
-    <row r="13" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
@@ -3018,45 +3128,54 @@
       <c r="AZ13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BA13" s="3" t="s">
+      <c r="BA13" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="BB13" s="4" t="s">
+      <c r="BB13" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="BC13" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="BD13" s="10"/>
+      <c r="BE13" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="BC13" s="10"/>
-      <c r="BE13" s="3" t="s">
+      <c r="BF13" s="10"/>
+      <c r="BH13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="BF13" s="3" t="s">
+      <c r="BI13" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="BG13" s="4" t="s">
+      <c r="BJ13" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="BH13" s="22"/>
-      <c r="BJ13" s="3" t="s">
+      <c r="BK13" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="BM13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BK13" s="3" t="s">
+      <c r="BN13" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="BL13" s="4" t="s">
+      <c r="BO13" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="BM13" s="22"/>
-      <c r="BO13" s="3" t="s">
+      <c r="BP13" s="22"/>
+      <c r="BR13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BP13" s="3" t="s">
+      <c r="BS13" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BQ13" s="4" t="s">
+      <c r="BT13" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="BR13" s="22"/>
+      <c r="BU13" s="22"/>
     </row>
-    <row r="14" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -3114,45 +3233,52 @@
       <c r="AZ14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BA14" s="3" t="s">
+      <c r="BA14" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="BB14" s="4" t="s">
+      <c r="BB14" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="BC14" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="BD14" s="10"/>
+      <c r="BE14" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="BC14" s="10"/>
-      <c r="BE14" s="3" t="s">
+      <c r="BF14" s="10"/>
+      <c r="BH14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BF14" s="3" t="s">
+      <c r="BI14" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="BG14" s="4" t="s">
+      <c r="BJ14" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="BH14" s="22"/>
-      <c r="BJ14" s="3" t="s">
+      <c r="BK14" s="10"/>
+      <c r="BM14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BK14" s="3" t="s">
+      <c r="BN14" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="BL14" s="4" t="s">
+      <c r="BO14" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="BM14" s="22"/>
-      <c r="BO14" s="3" t="s">
+      <c r="BP14" s="22"/>
+      <c r="BR14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BP14" s="3" t="s">
+      <c r="BS14" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="BQ14" s="4" t="s">
+      <c r="BT14" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="BR14" s="22"/>
+      <c r="BU14" s="22"/>
     </row>
-    <row r="15" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -3207,25 +3333,34 @@
       <c r="AZ15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BA15" s="3" t="s">
+      <c r="BA15" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="BB15" s="4" t="s">
+      <c r="BB15" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="BC15" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="BD15" s="10"/>
+      <c r="BE15" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="BC15" s="10"/>
-      <c r="BE15" s="3" t="s">
+      <c r="BF15" s="10"/>
+      <c r="BH15" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="BF15" s="3" t="s">
+      <c r="BI15" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="BG15" s="4" t="s">
+      <c r="BJ15" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="BH15" s="22"/>
+      <c r="BK15" s="26" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="16" spans="2:80" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -3279,18 +3414,20 @@
       <c r="AX16" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="BE16" s="3" t="s">
+      <c r="BH16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="BF16" s="3" t="s">
+      <c r="BI16" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="BG16" s="4" t="s">
+      <c r="BJ16" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="BH16" s="22"/>
+      <c r="BK16" s="26" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="17" spans="10:60" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:63" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J17" s="3" t="s">
         <v>25</v>
       </c>
@@ -3327,18 +3464,20 @@
       <c r="AX17" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="BE17" s="3" t="s">
+      <c r="BH17" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="BF17" s="3" t="s">
+      <c r="BI17" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="BG17" s="4" t="s">
+      <c r="BJ17" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="BH17" s="22"/>
+      <c r="BK17" s="26" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="18" spans="10:60" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J18" s="3" t="s">
         <v>26</v>
       </c>
@@ -3373,18 +3512,18 @@
         <v>225</v>
       </c>
       <c r="AX18" s="10"/>
-      <c r="BE18" s="3" t="s">
+      <c r="BH18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="BF18" s="3" t="s">
+      <c r="BI18" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="BG18" s="4" t="s">
+      <c r="BJ18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BH18" s="22"/>
+      <c r="BK18" s="10"/>
     </row>
-    <row r="19" spans="10:60" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J19" s="3" t="s">
         <v>27</v>
       </c>
@@ -3419,18 +3558,18 @@
         <v>224</v>
       </c>
       <c r="AX19" s="10"/>
-      <c r="BE19" s="3" t="s">
+      <c r="BH19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="BF19" s="3" t="s">
+      <c r="BI19" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="BG19" s="4" t="s">
+      <c r="BJ19" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="BH19" s="22"/>
+      <c r="BK19" s="10"/>
     </row>
-    <row r="20" spans="10:60" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J20" s="3" t="s">
         <v>28</v>
       </c>
@@ -3465,18 +3604,18 @@
         <v>115</v>
       </c>
       <c r="AX20" s="10"/>
-      <c r="BE20" s="3" t="s">
+      <c r="BH20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BF20" s="3" t="s">
+      <c r="BI20" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="BG20" s="4" t="s">
+      <c r="BJ20" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="BH20" s="22"/>
+      <c r="BK20" s="10"/>
     </row>
-    <row r="21" spans="10:60" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J21" s="3" t="s">
         <v>29</v>
       </c>
@@ -3511,18 +3650,18 @@
         <v>116</v>
       </c>
       <c r="AX21" s="10"/>
-      <c r="BE21" s="3" t="s">
+      <c r="BH21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BF21" s="3" t="s">
+      <c r="BI21" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="BG21" s="4" t="s">
+      <c r="BJ21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BH21" s="22"/>
+      <c r="BK21" s="10"/>
     </row>
-    <row r="22" spans="10:60" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J22" s="3" t="s">
         <v>30</v>
       </c>
@@ -3557,130 +3696,136 @@
         <v>117</v>
       </c>
       <c r="AX22" s="10"/>
-      <c r="BE22" s="3" t="s">
+      <c r="BH22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="BF22" s="3" t="s">
+      <c r="BI22" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="BG22" s="4" t="s">
+      <c r="BJ22" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="BH22" s="22"/>
+      <c r="BK22" s="10"/>
     </row>
-    <row r="23" spans="10:60" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE23" s="3" t="s">
+    <row r="23" spans="10:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH23" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="BF23" s="3" t="s">
+      <c r="BI23" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="BG23" s="4" t="s">
+      <c r="BJ23" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="BH23" s="22"/>
+      <c r="BK23" s="26" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="24" spans="10:60" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE24" s="3" t="s">
+    <row r="24" spans="10:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH24" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="BF24" s="3" t="s">
+      <c r="BI24" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="BG24" s="4" t="s">
+      <c r="BJ24" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="BH24" s="22"/>
+      <c r="BK24" s="26" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="25" spans="10:60" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE25" s="3" t="s">
+    <row r="25" spans="10:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH25" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="BF25" s="3" t="s">
+      <c r="BI25" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="BG25" s="4" t="s">
+      <c r="BJ25" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="BH25" s="22"/>
+      <c r="BK25" s="26" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="26" spans="10:60" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE26" s="3" t="s">
+    <row r="26" spans="10:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BF26" s="3" t="s">
+      <c r="BI26" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="BG26" s="4" t="s">
+      <c r="BJ26" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="BH26" s="22"/>
+      <c r="BK26" s="10"/>
     </row>
-    <row r="27" spans="10:60" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE27" s="3" t="s">
+    <row r="27" spans="10:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="BF27" s="3" t="s">
+      <c r="BI27" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="BG27" s="4" t="s">
+      <c r="BJ27" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="BH27" s="22"/>
+      <c r="BK27" s="10"/>
     </row>
-    <row r="28" spans="10:60" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE28" s="3" t="s">
+    <row r="28" spans="10:63" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BF28" s="3" t="s">
+      <c r="BI28" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="BG28" s="4" t="s">
+      <c r="BJ28" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="BH28" s="22"/>
+      <c r="BK28" s="10"/>
     </row>
-    <row r="29" spans="10:60" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE29" s="3" t="s">
+    <row r="29" spans="10:63" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BF29" s="3" t="s">
+      <c r="BI29" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BG29" s="4" t="s">
+      <c r="BJ29" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="BH29" s="22"/>
+      <c r="BK29" s="10"/>
     </row>
-    <row r="30" spans="10:60" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BE30" s="3" t="s">
+    <row r="30" spans="10:63" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BH30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BF30" s="3" t="s">
+      <c r="BI30" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="BG30" s="4" t="s">
+      <c r="BJ30" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="BH30" s="22"/>
+      <c r="BK30" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="AZ2:BE2"/>
+    <mergeCell ref="BH2:BJ2"/>
+    <mergeCell ref="R2:X2"/>
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AE2:AK2"/>
     <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="BY3:CA3"/>
-    <mergeCell ref="BT3:BV3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="AZ2:BB2"/>
-    <mergeCell ref="BE2:BG2"/>
-    <mergeCell ref="BJ2:BL2"/>
-    <mergeCell ref="BO2:BQ2"/>
-    <mergeCell ref="BT2:BV2"/>
-    <mergeCell ref="BY2:CA2"/>
-    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="CB3:CD3"/>
+    <mergeCell ref="BW3:BY3"/>
+    <mergeCell ref="BM2:BO2"/>
+    <mergeCell ref="BR2:BT2"/>
+    <mergeCell ref="BW2:BY2"/>
+    <mergeCell ref="CB2:CD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update remove item cart cart-item
</commit_message>
<xml_diff>
--- a/csdl-shopping-cart.xlsx
+++ b/csdl-shopping-cart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVMASTER\DEV2206LM_SpringBoot\shopping-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FDE70D-75F7-4A43-A519-4B892327666A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E00332A-B42B-4232-8F7C-B6FD54ED90B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91351D13-8343-4BE5-AE49-126D9A46B319}"/>
   </bookViews>
@@ -428,9 +428,6 @@
     <t>Mã thông báo duy nhất được liên kết với đơn đặt hàng để xác định nó qua nhiều phiên. Mã thông báo tương tự cũng có thể được chuyển đến Cổng thanh toán nếu được yêu cầu.</t>
   </si>
   <si>
-    <t>Trạng thái của đơn đặt hàng có thể là Mới, Đã thanh toán, Đã thanh toán, Không thành công, Đã vận chuyển, Đã giao, Đã trả lại và Hoàn thành.</t>
-  </si>
-  <si>
     <t>Tổng giá của các Mục đặt hàng.</t>
   </si>
   <si>
@@ -618,9 +615,6 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>Trạng thái của giỏ hàng có thể là Mới, Giỏ hàng, Thanh toán, Đã thanh toán, Hoàn thành và Bị bỏ rơi(New, Cart, Checkout, Paid, Complete, and Abandoned.).</t>
   </si>
   <si>
     <t>city</t>
@@ -959,6 +953,12 @@
   </si>
   <si>
     <t>Tổng giá của Đơn hàng đã bao gồm thuế và phí vận chuyển.</t>
+  </si>
+  <si>
+    <t>Trạng thái của giỏ hàng có thể là Mới=0, Giỏ hàng=1, Order=2, Đã thanh toán=3, và Bị bỏ rơi=4(New, Cart, Checkout, Paid, Complete, and Abandoned.).</t>
+  </si>
+  <si>
+    <t>Trạng thái của đơn đặt hàng có thể là Order=0, Chờ xác nhận, Đã thanh toán, Không thành công, Đã vận chuyển, Đã giao, Đã trả lại và Hoàn thành.</t>
   </si>
 </sst>
 </file>
@@ -1175,13 +1175,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1501,7 +1501,7 @@
   <dimension ref="B2:CE30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BO8" workbookViewId="0">
-      <selection activeCell="BU11" sqref="BU11"/>
+      <selection activeCell="BJ9" sqref="BJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1584,101 +1584,101 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:83" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="9"/>
+      <c r="J2" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="9"/>
+      <c r="R2" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Z2" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="9"/>
-      <c r="J2" s="31" t="s">
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AE2" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="9"/>
-      <c r="R2" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Z2" s="32" t="s">
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AM2" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AE2" s="31" t="s">
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="9"/>
+      <c r="AR2" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="31"/>
-      <c r="AM2" s="31" t="s">
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AZ2" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="9"/>
-      <c r="AR2" s="31" t="s">
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="9"/>
+      <c r="BH2" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="AS2" s="31"/>
-      <c r="AT2" s="31"/>
-      <c r="AU2" s="31"/>
-      <c r="AV2" s="31"/>
-      <c r="AW2" s="31"/>
-      <c r="AX2" s="31"/>
-      <c r="AZ2" s="31" t="s">
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="32"/>
+      <c r="BK2" s="9"/>
+      <c r="BM2" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="BA2" s="31"/>
-      <c r="BB2" s="31"/>
-      <c r="BC2" s="31"/>
-      <c r="BD2" s="31"/>
-      <c r="BE2" s="31"/>
-      <c r="BF2" s="9"/>
-      <c r="BH2" s="31" t="s">
+      <c r="BN2" s="32"/>
+      <c r="BO2" s="32"/>
+      <c r="BP2" s="9"/>
+      <c r="BR2" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="BI2" s="31"/>
-      <c r="BJ2" s="31"/>
-      <c r="BK2" s="9"/>
-      <c r="BM2" s="31" t="s">
+      <c r="BS2" s="32"/>
+      <c r="BT2" s="32"/>
+      <c r="BU2" s="9"/>
+      <c r="BW2" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="BX2" s="32"/>
+      <c r="BY2" s="32"/>
+      <c r="BZ2" s="9"/>
+      <c r="CB2" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="BN2" s="31"/>
-      <c r="BO2" s="31"/>
-      <c r="BP2" s="9"/>
-      <c r="BR2" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="BS2" s="31"/>
-      <c r="BT2" s="31"/>
-      <c r="BU2" s="9"/>
-      <c r="BW2" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="BX2" s="31"/>
-      <c r="BY2" s="31"/>
-      <c r="BZ2" s="9"/>
-      <c r="CB2" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="CC2" s="31"/>
-      <c r="CD2" s="31"/>
+      <c r="CC2" s="32"/>
+      <c r="CD2" s="32"/>
       <c r="CE2" s="9"/>
     </row>
     <row r="3" spans="2:83" x14ac:dyDescent="0.3">
@@ -1690,7 +1690,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H3" s="7"/>
       <c r="J3" s="7" t="s">
@@ -1701,7 +1701,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
       <c r="O3" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P3" s="7"/>
       <c r="R3" s="7" t="s">
@@ -1712,7 +1712,7 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X3" s="7"/>
       <c r="Z3" s="7" t="s">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AC3" s="7"/>
       <c r="AE3" s="7" t="s">
@@ -1731,15 +1731,15 @@
       <c r="AH3" s="12"/>
       <c r="AI3" s="12"/>
       <c r="AJ3" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AK3" s="7"/>
       <c r="AM3" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AN3" s="7"/>
       <c r="AO3" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AP3" s="7"/>
       <c r="AR3" s="7" t="s">
@@ -1750,7 +1750,7 @@
       <c r="AU3" s="12"/>
       <c r="AV3" s="12"/>
       <c r="AW3" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AX3" s="7"/>
       <c r="AZ3" s="7" t="s">
@@ -1761,7 +1761,7 @@
       <c r="BC3" s="12"/>
       <c r="BD3" s="12"/>
       <c r="BE3" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="BF3" s="7"/>
       <c r="BH3" s="8" t="s">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="BI3" s="8"/>
       <c r="BJ3" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BK3" s="8"/>
       <c r="BM3" s="7" t="s">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="BN3" s="7"/>
       <c r="BO3" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BP3" s="7"/>
       <c r="BR3" s="7" t="s">
@@ -1785,65 +1785,65 @@
       </c>
       <c r="BS3" s="7"/>
       <c r="BT3" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="BU3" s="7"/>
-      <c r="BW3" s="33" t="s">
+      <c r="BW3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="BX3" s="33"/>
-      <c r="BY3" s="33"/>
+      <c r="BX3" s="31"/>
+      <c r="BY3" s="31"/>
       <c r="BZ3" s="2"/>
-      <c r="CB3" s="33" t="s">
+      <c r="CB3" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="CC3" s="33"/>
-      <c r="CD3" s="33"/>
+      <c r="CC3" s="31"/>
+      <c r="CD3" s="31"/>
       <c r="CE3" s="2"/>
     </row>
     <row r="4" spans="2:83" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="18"/>
       <c r="C4" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
       <c r="R4" s="18"/>
       <c r="S4" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="T4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="W4" s="18"/>
       <c r="X4" s="21"/>
@@ -1853,16 +1853,16 @@
       <c r="AC4" s="21"/>
       <c r="AE4" s="18"/>
       <c r="AF4" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AG4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="AH4" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AI4" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AJ4" s="18"/>
       <c r="AK4" s="21"/>
@@ -1872,31 +1872,31 @@
       <c r="AP4" s="21"/>
       <c r="AR4" s="18"/>
       <c r="AS4" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AT4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="AU4" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AV4" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AW4" s="18"/>
       <c r="AX4" s="21"/>
       <c r="AZ4" s="18"/>
       <c r="BA4" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="BB4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="BC4" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="BD4" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="BE4" s="18"/>
       <c r="BF4" s="21"/>
@@ -1926,16 +1926,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>66</v>
@@ -1945,16 +1945,16 @@
         <v>0</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="O5" s="17" t="s">
         <v>73</v>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
@@ -1977,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="AA5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AB5" s="17" t="s">
         <v>91</v>
@@ -1987,16 +1987,16 @@
         <v>0</v>
       </c>
       <c r="AF5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AG5" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AI5" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AJ5" s="17" t="s">
         <v>99</v>
@@ -2006,26 +2006,26 @@
         <v>0</v>
       </c>
       <c r="AN5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AO5" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AP5" s="10"/>
       <c r="AR5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="AS5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AT5" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AU5" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AV5" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AW5" s="17" t="s">
         <v>106</v>
@@ -2035,16 +2035,16 @@
         <v>0</v>
       </c>
       <c r="BA5" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BB5" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BC5" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BD5" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="BE5" s="17" t="s">
         <v>116</v>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="BI5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BJ5" s="17" t="s">
         <v>126</v>
@@ -2064,27 +2064,27 @@
         <v>0</v>
       </c>
       <c r="BN5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BO5" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BP5" s="22"/>
       <c r="BR5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="BS5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BT5" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BU5" s="22"/>
       <c r="BW5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="BX5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BY5" s="14"/>
       <c r="BZ5" s="24"/>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="CC5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="CD5" s="14"/>
       <c r="CE5" s="24"/>
@@ -2102,13 +2102,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="4" t="s">
@@ -2119,16 +2119,16 @@
         <v>12</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>74</v>
@@ -2138,7 +2138,7 @@
         <v>31</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -2151,7 +2151,7 @@
         <v>31</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AB6" s="4" t="s">
         <v>88</v>
@@ -2161,7 +2161,7 @@
         <v>34</v>
       </c>
       <c r="AF6" s="25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="AG6" s="26"/>
       <c r="AH6" s="26"/>
@@ -2170,13 +2170,13 @@
         <v>100</v>
       </c>
       <c r="AK6" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AM6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AO6" s="4" t="s">
         <v>104</v>
@@ -2186,16 +2186,16 @@
         <v>12</v>
       </c>
       <c r="AS6" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AT6" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AU6" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV6" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AW6" s="4" t="s">
         <v>107</v>
@@ -2205,16 +2205,16 @@
         <v>31</v>
       </c>
       <c r="BA6" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="BB6" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BC6" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="BD6" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="BE6" s="4" t="s">
         <v>117</v>
@@ -2224,7 +2224,7 @@
         <v>12</v>
       </c>
       <c r="BI6" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BJ6" s="4" t="s">
         <v>127</v>
@@ -2234,27 +2234,27 @@
         <v>31</v>
       </c>
       <c r="BN6" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="BO6" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BP6" s="22"/>
       <c r="BR6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="BS6" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BT6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="BU6" s="22"/>
       <c r="BW6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="BX6" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="BY6" s="3"/>
       <c r="BZ6" s="24"/>
@@ -2262,7 +2262,7 @@
         <v>13</v>
       </c>
       <c r="CC6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="CD6" s="3"/>
       <c r="CE6" s="24"/>
@@ -2272,30 +2272,30 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H7" s="3"/>
       <c r="J7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="4" t="s">
@@ -2306,7 +2306,7 @@
         <v>32</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -2319,7 +2319,7 @@
         <v>34</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="AB7" s="4" t="s">
         <v>92</v>
@@ -2329,13 +2329,13 @@
         <v>13</v>
       </c>
       <c r="AF7" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AG7" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AH7" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AI7" s="10"/>
       <c r="AJ7" s="4" t="s">
@@ -2346,7 +2346,7 @@
         <v>38</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AO7" s="4" t="s">
         <v>105</v>
@@ -2356,35 +2356,35 @@
         <v>40</v>
       </c>
       <c r="AS7" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AT7" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AU7" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AV7" s="26"/>
       <c r="AW7" s="27" t="s">
         <v>108</v>
       </c>
       <c r="AX7" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AZ7" s="3" t="s">
         <v>48</v>
       </c>
       <c r="BA7" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BB7" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BC7" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="BD7" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="BD7" s="10" t="s">
-        <v>290</v>
       </c>
       <c r="BE7" s="4" t="s">
         <v>118</v>
@@ -2394,39 +2394,39 @@
         <v>48</v>
       </c>
       <c r="BI7" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BJ7" s="4" t="s">
         <v>128</v>
       </c>
       <c r="BK7" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="BM7" s="3" t="s">
         <v>58</v>
       </c>
       <c r="BN7" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="BO7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BP7" s="22"/>
       <c r="BR7" s="3" t="s">
         <v>58</v>
       </c>
       <c r="BS7" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="BT7" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BU7" s="22"/>
       <c r="BW7" s="3" t="s">
         <v>64</v>
       </c>
       <c r="BX7" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BY7" s="3"/>
       <c r="BZ7" s="24"/>
@@ -2434,7 +2434,7 @@
         <v>14</v>
       </c>
       <c r="CC7" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CD7" s="3"/>
       <c r="CE7" s="24"/>
@@ -2444,16 +2444,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>68</v>
@@ -2463,26 +2463,26 @@
         <v>14</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N8" s="26"/>
       <c r="O8" s="27" t="s">
         <v>76</v>
       </c>
       <c r="P8" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -2495,7 +2495,7 @@
         <v>13</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AB8" s="4" t="s">
         <v>93</v>
@@ -2505,13 +2505,13 @@
         <v>14</v>
       </c>
       <c r="AF8" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AG8" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AH8" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AI8" s="26"/>
       <c r="AJ8" s="27" t="s">
@@ -2522,32 +2522,32 @@
         <v>41</v>
       </c>
       <c r="AS8" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AT8" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AU8" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AV8" s="26"/>
       <c r="AW8" s="27" t="s">
         <v>109</v>
       </c>
       <c r="AX8" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AZ8" s="25" t="s">
         <v>19</v>
       </c>
       <c r="BA8" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="BB8" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="BC8" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="BD8" s="26"/>
       <c r="BE8" s="27" t="s">
@@ -2558,19 +2558,19 @@
         <v>41</v>
       </c>
       <c r="BI8" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="BJ8" s="27" t="s">
         <v>129</v>
       </c>
       <c r="BK8" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="BM8" s="25" t="s">
         <v>19</v>
       </c>
       <c r="BN8" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="BO8" s="27" t="s">
         <v>119</v>
@@ -2580,36 +2580,36 @@
         <v>61</v>
       </c>
       <c r="BS8" s="25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="BT8" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BU8" s="22"/>
       <c r="CB8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="CC8" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CD8" s="3"/>
       <c r="CE8" s="24"/>
     </row>
-    <row r="9" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:83" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>69</v>
@@ -2619,16 +2619,16 @@
         <v>15</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>16</v>
@@ -2638,7 +2638,7 @@
         <v>35</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB9" s="4" t="s">
         <v>94</v>
@@ -2648,13 +2648,13 @@
         <v>15</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AG9" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AH9" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AI9" s="10"/>
       <c r="AJ9" s="4" t="s">
@@ -2665,30 +2665,30 @@
         <v>42</v>
       </c>
       <c r="AS9" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AT9" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AU9" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AV9" s="10"/>
       <c r="AW9" s="4" t="s">
-        <v>194</v>
+        <v>303</v>
       </c>
       <c r="AX9" s="10"/>
       <c r="AZ9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BA9" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BB9" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="BC9" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BD9" s="10"/>
       <c r="BE9" s="4" t="s">
@@ -2699,17 +2699,17 @@
         <v>42</v>
       </c>
       <c r="BI9" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BJ9" s="4" t="s">
-        <v>130</v>
+        <v>304</v>
       </c>
       <c r="BK9" s="10"/>
       <c r="BM9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BN9" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BO9" s="4" t="s">
         <v>120</v>
@@ -2719,50 +2719,50 @@
         <v>18</v>
       </c>
       <c r="BS9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BT9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BU9" s="22"/>
       <c r="CB9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="CC9" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CD9" s="3"/>
       <c r="CE9" s="24"/>
     </row>
     <row r="10" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H10" s="3"/>
       <c r="J10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="4" t="s">
@@ -2773,7 +2773,7 @@
         <v>36</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB10" s="4" t="s">
         <v>95</v>
@@ -2783,13 +2783,13 @@
         <v>29</v>
       </c>
       <c r="AF10" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AG10" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="AH10" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="AH10" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="AI10" s="10"/>
       <c r="AJ10" s="4" t="s">
@@ -2800,13 +2800,13 @@
         <v>1</v>
       </c>
       <c r="AS10" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AT10" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU10" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV10" s="10"/>
       <c r="AW10" s="4" t="s">
@@ -2817,13 +2817,13 @@
         <v>21</v>
       </c>
       <c r="BA10" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BB10" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="BC10" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BD10" s="10"/>
       <c r="BE10" s="4" t="s">
@@ -2834,17 +2834,17 @@
         <v>51</v>
       </c>
       <c r="BI10" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="BJ10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="BK10" s="10"/>
       <c r="BM10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="BN10" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BO10" s="4" t="s">
         <v>121</v>
@@ -2854,10 +2854,10 @@
         <v>62</v>
       </c>
       <c r="BS10" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="BT10" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="BU10" s="22"/>
     </row>
@@ -2866,45 +2866,45 @@
         <v>5</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="27" t="s">
         <v>78</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AB11" s="4" t="s">
         <v>96</v>
@@ -2914,30 +2914,30 @@
         <v>2</v>
       </c>
       <c r="AS11" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AT11" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU11" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV11" s="10"/>
       <c r="AW11" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AX11" s="10"/>
       <c r="AZ11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="BA11" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BB11" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="BC11" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BD11" s="10"/>
       <c r="BE11" s="4" t="s">
@@ -2948,17 +2948,17 @@
         <v>52</v>
       </c>
       <c r="BI11" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="BJ11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BK11" s="10"/>
       <c r="BM11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="BN11" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BO11" s="4" t="s">
         <v>122</v>
@@ -2968,10 +2968,10 @@
         <v>42</v>
       </c>
       <c r="BS11" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BT11" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="BU11" s="22"/>
     </row>
@@ -2980,43 +2980,43 @@
         <v>6</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="27" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H12" s="25"/>
       <c r="J12" s="25" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N12" s="26"/>
       <c r="O12" s="27" t="s">
         <v>79</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AB12" s="4" t="s">
         <v>97</v>
@@ -3026,13 +3026,13 @@
         <v>3</v>
       </c>
       <c r="AS12" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AT12" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU12" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AV12" s="10"/>
       <c r="AW12" s="4" t="s">
@@ -3043,81 +3043,81 @@
         <v>49</v>
       </c>
       <c r="BA12" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BB12" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BC12" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BD12" s="10"/>
       <c r="BE12" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BF12" s="10"/>
       <c r="BH12" s="25" t="s">
         <v>53</v>
       </c>
       <c r="BI12" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BJ12" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BK12" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="BM12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="BN12" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BO12" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BP12" s="22"/>
       <c r="BR12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="BS12" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="BT12" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BU12" s="22"/>
     </row>
     <row r="13" spans="2:83" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="27" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H13" s="25"/>
       <c r="J13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="4" t="s">
@@ -3128,7 +3128,7 @@
         <v>29</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AB13" s="4" t="s">
         <v>98</v>
@@ -3138,13 +3138,13 @@
         <v>4</v>
       </c>
       <c r="AS13" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AT13" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU13" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AV13" s="10"/>
       <c r="AW13" s="4" t="s">
@@ -3155,13 +3155,13 @@
         <v>24</v>
       </c>
       <c r="BA13" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="BB13" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BC13" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="BD13" s="10"/>
       <c r="BE13" s="4" t="s">
@@ -3172,32 +3172,32 @@
         <v>54</v>
       </c>
       <c r="BI13" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BJ13" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BK13" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="BM13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="BN13" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BO13" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BP13" s="22"/>
       <c r="BR13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="BS13" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BT13" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BU13" s="22"/>
     </row>
@@ -3206,13 +3206,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="27" t="s">
@@ -3223,17 +3223,17 @@
         <v>21</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P14" s="10"/>
       <c r="AC14" s="10"/>
@@ -3241,32 +3241,32 @@
         <v>43</v>
       </c>
       <c r="AS14" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AT14" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU14" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV14" s="10"/>
       <c r="AW14" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AX14" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AZ14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="BA14" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BB14" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BC14" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="BD14" s="10"/>
       <c r="BE14" s="4" t="s">
@@ -3277,30 +3277,30 @@
         <v>55</v>
       </c>
       <c r="BI14" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="BJ14" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BK14" s="10"/>
       <c r="BM14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="BN14" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BO14" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BP14" s="22"/>
       <c r="BR14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="BS14" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BT14" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU14" s="22"/>
     </row>
@@ -3309,13 +3309,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="4" t="s">
@@ -3326,13 +3326,13 @@
         <v>22</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L15" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="M15" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>278</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="4" t="s">
@@ -3343,13 +3343,13 @@
         <v>44</v>
       </c>
       <c r="AS15" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AT15" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU15" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV15" s="26"/>
       <c r="AW15" s="27" t="s">
@@ -3360,13 +3360,13 @@
         <v>29</v>
       </c>
       <c r="BA15" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BB15" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="BC15" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="BC15" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="BD15" s="10"/>
       <c r="BE15" s="4" t="s">
@@ -3377,13 +3377,13 @@
         <v>56</v>
       </c>
       <c r="BI15" s="25" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BJ15" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK15" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="2:83" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3391,13 +3391,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="4" t="s">
@@ -3408,63 +3408,63 @@
         <v>23</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N16" s="10"/>
       <c r="O16" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="P16" s="10"/>
       <c r="AR16" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AS16" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AT16" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU16" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV16" s="26"/>
       <c r="AW16" s="27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AX16" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="BH16" s="25" t="s">
         <v>21</v>
       </c>
       <c r="BI16" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BJ16" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BK16" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="2:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="4" t="s">
@@ -3475,13 +3475,13 @@
         <v>24</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="4" t="s">
@@ -3489,64 +3489,64 @@
       </c>
       <c r="P17" s="10"/>
       <c r="AR17" s="25" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AS17" s="25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AT17" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU17" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV17" s="26"/>
       <c r="AW17" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AX17" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="BH17" s="25" t="s">
         <v>57</v>
       </c>
       <c r="BI17" s="25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="BJ17" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BK17" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="2:63" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>300</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H18" s="3"/>
       <c r="J18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="4" t="s">
@@ -3557,24 +3557,24 @@
         <v>45</v>
       </c>
       <c r="AS18" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AT18" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU18" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV18" s="10"/>
       <c r="AW18" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AX18" s="10"/>
       <c r="BH18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="BI18" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="BJ18" s="4" t="s">
         <v>67</v>
@@ -3586,44 +3586,44 @@
         <v>26</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M19" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N19" s="26"/>
       <c r="O19" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P19" s="10"/>
       <c r="AR19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="AS19" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AT19" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AU19" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV19" s="10"/>
       <c r="AW19" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AX19" s="10"/>
       <c r="BH19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="BI19" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="BJ19" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BK19" s="10"/>
     </row>
@@ -3632,13 +3632,13 @@
         <v>27</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N20" s="26"/>
       <c r="O20" s="27" t="s">
@@ -3649,13 +3649,13 @@
         <v>24</v>
       </c>
       <c r="AS20" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AT20" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AU20" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AV20" s="10"/>
       <c r="AW20" s="4" t="s">
@@ -3666,7 +3666,7 @@
         <v>3</v>
       </c>
       <c r="BI20" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BJ20" s="4" t="s">
         <v>110</v>
@@ -3678,13 +3678,13 @@
         <v>28</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N21" s="10"/>
       <c r="O21" s="4" t="s">
@@ -3695,13 +3695,13 @@
         <v>25</v>
       </c>
       <c r="AS21" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AT21" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AU21" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AV21" s="10"/>
       <c r="AW21" s="4" t="s">
@@ -3712,7 +3712,7 @@
         <v>4</v>
       </c>
       <c r="BI21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BJ21" s="4" t="s">
         <v>111</v>
@@ -3724,13 +3724,13 @@
         <v>29</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L22" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="M22" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="N22" s="10"/>
       <c r="O22" s="4" t="s">
@@ -3741,13 +3741,13 @@
         <v>29</v>
       </c>
       <c r="AS22" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AT22" s="10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AU22" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AV22" s="10"/>
       <c r="AW22" s="4" t="s">
@@ -3758,10 +3758,10 @@
         <v>43</v>
       </c>
       <c r="BI22" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="BJ22" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="BK22" s="10"/>
     </row>
@@ -3770,41 +3770,41 @@
         <v>44</v>
       </c>
       <c r="BI23" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="BJ23" s="27" t="s">
         <v>112</v>
       </c>
       <c r="BK23" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="2:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BH24" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="BI24" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="BJ24" s="27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="BK24" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="2:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="BH25" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="BI25" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="BJ25" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="BI25" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="BJ25" s="27" t="s">
-        <v>216</v>
-      </c>
       <c r="BK25" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="2:63" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3812,10 +3812,10 @@
         <v>45</v>
       </c>
       <c r="BI26" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="BJ26" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="BK26" s="10"/>
     </row>
@@ -3824,10 +3824,10 @@
         <v>46</v>
       </c>
       <c r="BI27" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="BJ27" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="BK27" s="10"/>
     </row>
@@ -3836,10 +3836,10 @@
         <v>24</v>
       </c>
       <c r="BI28" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="BJ28" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BK28" s="10"/>
     </row>
@@ -3848,10 +3848,10 @@
         <v>25</v>
       </c>
       <c r="BI29" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BJ29" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BK29" s="10"/>
     </row>
@@ -3860,21 +3860,15 @@
         <v>29</v>
       </c>
       <c r="BI30" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BJ30" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BK30" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="CB3:CD3"/>
-    <mergeCell ref="BW3:BY3"/>
-    <mergeCell ref="BM2:BO2"/>
-    <mergeCell ref="BR2:BT2"/>
-    <mergeCell ref="BW2:BY2"/>
-    <mergeCell ref="CB2:CD2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="AM2:AO2"/>
@@ -3884,6 +3878,12 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AE2:AK2"/>
     <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="CB3:CD3"/>
+    <mergeCell ref="BW3:BY3"/>
+    <mergeCell ref="BM2:BO2"/>
+    <mergeCell ref="BR2:BT2"/>
+    <mergeCell ref="BW2:BY2"/>
+    <mergeCell ref="CB2:CD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update set status order, set user, category
</commit_message>
<xml_diff>
--- a/csdl-shopping-cart.xlsx
+++ b/csdl-shopping-cart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVMASTER\DEV2206LM_SpringBoot\shopping-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FE5532-2437-468A-9065-B599AB316E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28819561-A600-4E1C-9FB4-5D4962A9B229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91351D13-8343-4BE5-AE49-126D9A46B319}"/>
   </bookViews>
@@ -996,7 +996,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,6 +1030,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1089,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1175,14 +1187,38 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1500,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E867DBF7-62FE-4C81-BE5B-4B051B3412A0}">
   <dimension ref="B2:CE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1584,101 +1620,101 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:83" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="9"/>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="9"/>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Z2" s="33" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Z2" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AE2" s="32" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AE2" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AM2" s="32" t="s">
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AM2" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
       <c r="AP2" s="9"/>
-      <c r="AR2" s="32" t="s">
+      <c r="AR2" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AZ2" s="32" t="s">
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
+      <c r="AW2" s="31"/>
+      <c r="AX2" s="31"/>
+      <c r="AZ2" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="BA2" s="32"/>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
+      <c r="BA2" s="31"/>
+      <c r="BB2" s="31"/>
+      <c r="BC2" s="31"/>
+      <c r="BD2" s="31"/>
+      <c r="BE2" s="31"/>
       <c r="BF2" s="9"/>
-      <c r="BH2" s="32" t="s">
+      <c r="BH2" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="BI2" s="32"/>
-      <c r="BJ2" s="32"/>
+      <c r="BI2" s="31"/>
+      <c r="BJ2" s="31"/>
       <c r="BK2" s="9"/>
-      <c r="BM2" s="32" t="s">
+      <c r="BM2" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="BN2" s="32"/>
-      <c r="BO2" s="32"/>
+      <c r="BN2" s="31"/>
+      <c r="BO2" s="31"/>
       <c r="BP2" s="9"/>
-      <c r="BR2" s="32" t="s">
+      <c r="BR2" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="BS2" s="32"/>
-      <c r="BT2" s="32"/>
+      <c r="BS2" s="31"/>
+      <c r="BT2" s="31"/>
       <c r="BU2" s="9"/>
-      <c r="BW2" s="32" t="s">
+      <c r="BW2" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="BX2" s="32"/>
-      <c r="BY2" s="32"/>
+      <c r="BX2" s="31"/>
+      <c r="BY2" s="31"/>
       <c r="BZ2" s="9"/>
-      <c r="CB2" s="32" t="s">
+      <c r="CB2" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="CC2" s="32"/>
-      <c r="CD2" s="32"/>
+      <c r="CC2" s="31"/>
+      <c r="CD2" s="31"/>
       <c r="CE2" s="9"/>
     </row>
     <row r="3" spans="2:83" x14ac:dyDescent="0.3">
@@ -1788,17 +1824,17 @@
         <v>207</v>
       </c>
       <c r="BU3" s="7"/>
-      <c r="BW3" s="31" t="s">
+      <c r="BW3" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="BX3" s="31"/>
-      <c r="BY3" s="31"/>
+      <c r="BX3" s="33"/>
+      <c r="BY3" s="33"/>
       <c r="BZ3" s="2"/>
-      <c r="CB3" s="31" t="s">
+      <c r="CB3" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="CC3" s="31"/>
-      <c r="CD3" s="31"/>
+      <c r="CC3" s="33"/>
+      <c r="CD3" s="33"/>
       <c r="CE3" s="2"/>
     </row>
     <row r="4" spans="2:83" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2976,23 +3012,23 @@
       <c r="BU11" s="22"/>
     </row>
     <row r="12" spans="2:83" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="39" t="s">
         <v>257</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27" t="s">
+      <c r="F12" s="40"/>
+      <c r="G12" s="41" t="s">
         <v>293</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="38"/>
       <c r="J12" s="25" t="s">
         <v>19</v>
       </c>
@@ -3090,23 +3126,23 @@
       <c r="BU12" s="22"/>
     </row>
     <row r="13" spans="2:83" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="34" t="s">
         <v>290</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="34"/>
       <c r="J13" s="3" t="s">
         <v>20</v>
       </c>
@@ -3869,6 +3905,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="CB3:CD3"/>
+    <mergeCell ref="BW3:BY3"/>
+    <mergeCell ref="BM2:BO2"/>
+    <mergeCell ref="BR2:BT2"/>
+    <mergeCell ref="BW2:BY2"/>
+    <mergeCell ref="CB2:CD2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="AM2:AO2"/>
@@ -3878,12 +3920,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AE2:AK2"/>
     <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="CB3:CD3"/>
-    <mergeCell ref="BW3:BY3"/>
-    <mergeCell ref="BM2:BO2"/>
-    <mergeCell ref="BR2:BT2"/>
-    <mergeCell ref="BW2:BY2"/>
-    <mergeCell ref="CB2:CD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>